<commit_message>
Update package add custom action menu with listener
</commit_message>
<xml_diff>
--- a/Docs/TaskLists.xlsx
+++ b/Docs/TaskLists.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Add actionbars at surah activity</t>
   </si>
@@ -55,13 +56,44 @@
   </si>
   <si>
     <t xml:space="preserve">Add max repeat popup </t>
+  </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a verse </t>
+  </si>
+  <si>
+    <t>Loop the verse Max loop time</t>
+  </si>
+  <si>
+    <t>After finish loop the next verse</t>
+  </si>
+  <si>
+    <t>Post action</t>
+  </si>
+  <si>
+    <t>Expected output</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Repeat on
+Max loop count = 5</t>
+  </si>
+  <si>
+    <t>Actual Output</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +101,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -86,14 +130,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -447,4 +612,920 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="35.85546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>